<commit_message>
Fixing references in Form-4SF
</commit_message>
<xml_diff>
--- a/forms/Form-4SF.xlsx
+++ b/forms/Form-4SF.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\Data dissemination\iotc-reference-data\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CE1784-5B39-444B-9A4D-2E4FAB192A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079045DD-758C-4D64-88A2-71D015135145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="jbPe6SBLf4oG4Cgxdp2GTHPCnTakxOLusQvs3FLR97ZGw7ZrHwFP80gs+fK1zVtwmXmlsYM45w/LTktaEDAlHA==" workbookSaltValue="+e6btQraNKSRCi9yKssXHA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
@@ -672,7 +672,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -817,6 +817,23 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -857,24 +874,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1210,24 +1209,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="56"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="61"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="57"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -1277,15 +1276,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="53"/>
+      <c r="D8" s="58"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="53" t="s">
+      <c r="F8" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="53"/>
+      <c r="G8" s="58"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1308,7 +1307,7 @@
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="10" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="22"/>
@@ -1390,7 +1389,7 @@
       </c>
       <c r="D18" s="36"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="67" t="s">
+      <c r="F18" s="53" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="36"/>
@@ -1398,12 +1397,12 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="53" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="36"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="67" t="s">
+      <c r="F19" s="53" t="s">
         <v>20</v>
       </c>
       <c r="G19" s="36"/>
@@ -1411,7 +1410,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="53" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="36"/>
@@ -1454,20 +1453,20 @@
       <c r="C24" s="12"/>
       <c r="D24" s="15"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="53" t="s">
+      <c r="F24" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="53"/>
+      <c r="G24" s="58"/>
       <c r="H24" s="11"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="53" t="s">
         <v>38</v>
       </c>
       <c r="D25" s="36"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="67" t="s">
+      <c r="F25" s="53" t="s">
         <v>21</v>
       </c>
       <c r="G25" s="36"/>
@@ -1478,7 +1477,7 @@
       <c r="C26" s="12"/>
       <c r="D26" s="15"/>
       <c r="E26" s="10"/>
-      <c r="F26" s="67" t="s">
+      <c r="F26" s="53" t="s">
         <v>41</v>
       </c>
       <c r="G26" s="36"/>
@@ -1486,12 +1485,12 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="53" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="36"/>
       <c r="E27" s="10"/>
-      <c r="F27" s="67" t="s">
+      <c r="F27" s="53" t="s">
         <v>22</v>
       </c>
       <c r="G27" s="36"/>
@@ -1499,7 +1498,7 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="9"/>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="36"/>
@@ -1512,7 +1511,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="9"/>
-      <c r="C29" s="67" t="s">
+      <c r="C29" s="53" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="36"/>
@@ -1523,12 +1522,12 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
-      <c r="C30" s="67" t="s">
+      <c r="C30" s="53" t="s">
         <v>30</v>
       </c>
       <c r="D30" s="36"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="67" t="s">
+      <c r="F30" s="53" t="s">
         <v>42</v>
       </c>
       <c r="G30" s="36"/>
@@ -1543,7 +1542,7 @@
       <c r="E31" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="67" t="s">
+      <c r="F31" s="53" t="s">
         <v>35</v>
       </c>
       <c r="G31" s="36"/>
@@ -1589,11 +1588,11 @@
     </row>
     <row r="36" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="9"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="62"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="67"/>
       <c r="H36" s="11"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1610,7 +1609,7 @@
       <c r="D38" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="7Exm+1JjaLpBZ4qqnrLA2+IIPThLibpHMx8XXZtIJWE9M4I21dfNciFGOhntHoBoe6L7mcjwZOXXVmW4F+/Jig==" saltValue="V5mEvdI4JJo7w9SaQSk8dA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="6V1Wn76De8eW/mCIZJ7wIAW4MCo0r+B32r2Io1HirUsYP76Cylk/Mz+XhCr48uJrQtQ/e8dtQi8/o46sqL3OTQ==" saltValue="1k/9AjWaL2HctrhQGqJ2dg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="5">
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="F8:G8"/>
@@ -1676,46 +1675,46 @@
       <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="56"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="61"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="57"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
     </row>
     <row r="4" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="63" t="s">
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="65"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="70"/>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="55" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="38" t="s">
@@ -1724,10 +1723,10 @@
       <c r="F5" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="70" t="s">
+      <c r="G5" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="71" t="s">
+      <c r="H5" s="57" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>